<commit_message>
update data requirements input file
</commit_message>
<xml_diff>
--- a/inputs/data/DataRequirements.xlsx
+++ b/inputs/data/DataRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfernandez diaz\Documents\DATA SECTION\Meetings\iotc-wpdcs-data\inputs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfernandez diaz\Documents\DATA SECTION\Data reporting guidelines\data-reporting-guidelines\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DC79CA-2F98-4BEF-B471-9428E005782A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3051D769-D761-4B8B-930F-6A3F02FCED38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6F15DFC0-4881-4B41-93EC-8690959E7BCB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F15DFC0-4881-4B41-93EC-8690959E7BCB}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
   <si>
     <t>Industrial fleets</t>
   </si>
@@ -190,28 +190,16 @@
     <t>Longline and surface fisheries</t>
   </si>
   <si>
-    <t>3AR, 3CE, 3SU</t>
-  </si>
-  <si>
     <t>Effort by fishery, school type, grid area and month strata, including supply vessels</t>
   </si>
   <si>
-    <t>3FA</t>
-  </si>
-  <si>
     <t>15/02, 19/02</t>
   </si>
   <si>
-    <t>3AR, 3CE, 3FA</t>
-  </si>
-  <si>
     <t>Interactions with drifting floating objects by purse seiners and supply vessels, including number of sets by 1° grid area and month strata</t>
   </si>
   <si>
     <t>19/02</t>
-  </si>
-  <si>
-    <t>3BU</t>
   </si>
   <si>
     <t>Daily positions of active buoys equipping FADs and natural floating objects, by purse seine vessel</t>
@@ -584,24 +572,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25017514-967B-472A-9209-0CA7A44FB208}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.81640625" customWidth="1"/>
-    <col min="6" max="6" width="61.7265625" customWidth="1"/>
-    <col min="7" max="7" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -611,18 +598,15 @@
       <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -632,18 +616,15 @@
       <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -653,18 +634,15 @@
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -674,18 +652,15 @@
       <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="37.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -695,18 +670,15 @@
       <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -716,18 +688,15 @@
       <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -737,17 +706,14 @@
       <c r="C7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>54</v>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -757,57 +723,48 @@
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>57</v>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -817,37 +774,31 @@
       <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -857,13 +808,10 @@
       <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>30</v>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -881,18 +829,18 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.81640625" customWidth="1"/>
-    <col min="6" max="6" width="56.26953125" customWidth="1"/>
-    <col min="7" max="7" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -913,7 +861,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -934,7 +882,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -955,7 +903,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -976,7 +924,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -996,7 +944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1016,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1036,7 +984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1056,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>